<commit_message>
Segundo guardado del proyecto.
</commit_message>
<xml_diff>
--- a/Himnos 2025 marzo.xlsx
+++ b/Himnos 2025 marzo.xlsx
@@ -243,7 +243,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="149">
   <si>
     <t>Opcionales</t>
   </si>
@@ -706,6 +706,9 @@
   </si>
   <si>
     <t>DOMINGO 30 T</t>
+  </si>
+  <si>
+    <t>Alma, Bendice ah Seños</t>
   </si>
 </sst>
 </file>
@@ -2382,8 +2385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N34" sqref="N34:R40"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2505,7 +2508,7 @@
         <v>1</v>
       </c>
       <c r="I3" s="237" t="s">
-        <v>120</v>
+        <v>148</v>
       </c>
       <c r="J3" s="244">
         <v>234</v>

</xml_diff>